<commit_message>
Added info for user
</commit_message>
<xml_diff>
--- a/patternSystems/genericTools/Generic Measurement Subdivision Table.xlsx
+++ b/patternSystems/genericTools/Generic Measurement Subdivision Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Programming Projects\InterpolationDraping\InterpolationDraping\patternSystems\genericTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BD45E1-A1C9-422B-8943-7A1512EEFC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8934CE13-3A22-4B31-B3B8-5F26C0CC6033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
   <si>
     <t>This Excel sheet is designed to assist in pattern drafting by providing a table of partial measurements (1/2 breast, 1/3 breast, etc.) for drafting out of older books.</t>
   </si>
@@ -183,6 +183,112 @@
   <si>
     <t>Like the tables above, these tables currently round to the nearest tenth of a centimeter, and may not add back to the original length.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Half Length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tables are useful for measurements like the breast measure, duplicated across the left and right side.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Full Length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tables are useful for measurements like height, which match the measurement to the panel.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There are two types of tables: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Half Lengths</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Full Length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +296,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="#\ ?/8"/>
+    <numFmt numFmtId="165" formatCode="#\ ?/8"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -848,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -901,55 +1007,56 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Z128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1271,26 +1378,35 @@
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F6" s="83" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -1327,42 +1443,42 @@
       <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="44">
         <v>38</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="45">
         <v>0.5</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="46">
         <f>C16+D16</f>
         <v>38.5</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="47">
         <f>E16/2</f>
         <v>19.25</v>
       </c>
-      <c r="G16" s="60">
+      <c r="G16" s="48">
         <f>F16/2</f>
         <v>9.625</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="49">
         <f>F16/3</f>
         <v>6.416666666666667</v>
       </c>
-      <c r="I16" s="60">
+      <c r="I16" s="48">
         <f>F16/4</f>
         <v>4.8125</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="66"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
@@ -1449,1030 +1565,1032 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
-      <c r="C29" s="78">
+      <c r="C29" s="66">
         <v>38</v>
       </c>
-      <c r="D29" s="57">
+      <c r="D29" s="45">
         <v>0.5</v>
       </c>
-      <c r="E29" s="58">
+      <c r="E29" s="46">
         <f>C29+D29</f>
         <v>38.5</v>
       </c>
-      <c r="F29" s="59">
+      <c r="F29" s="47">
         <f>E29/2</f>
         <v>19.25</v>
       </c>
-      <c r="G29" s="60">
+      <c r="G29" s="48">
         <f>F29/2</f>
         <v>9.625</v>
       </c>
-      <c r="H29" s="61">
+      <c r="H29" s="49">
         <f>F29/3</f>
         <v>6.416666666666667</v>
       </c>
-      <c r="I29" s="60">
+      <c r="I29" s="48">
         <f>F29/4</f>
         <v>4.8125</v>
       </c>
-      <c r="J29" s="61">
+      <c r="J29" s="49">
         <f>F29/5</f>
         <v>3.85</v>
       </c>
-      <c r="K29" s="61">
+      <c r="K29" s="49">
         <f>F29/6</f>
         <v>3.2083333333333335</v>
       </c>
-      <c r="L29" s="61">
+      <c r="L29" s="49">
         <f>F29/7</f>
         <v>2.75</v>
       </c>
-      <c r="M29" s="60">
+      <c r="M29" s="48">
         <f>F29/8</f>
         <v>2.40625</v>
       </c>
-      <c r="N29" s="61">
+      <c r="N29" s="49">
         <f>F29/9</f>
         <v>2.1388888888888888</v>
       </c>
-      <c r="O29" s="61">
+      <c r="O29" s="49">
         <f>F29/10</f>
         <v>1.925</v>
       </c>
-      <c r="P29" s="61">
+      <c r="P29" s="49">
         <f>F29/11</f>
         <v>1.75</v>
       </c>
-      <c r="Q29" s="67">
+      <c r="Q29" s="55">
         <f>F29/12</f>
         <v>1.6041666666666667</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" s="11"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="58">
+      <c r="C30" s="56">
+        <v>36</v>
+      </c>
+      <c r="D30" s="57"/>
+      <c r="E30" s="46">
         <f>C30+D30</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="59">
+        <v>36</v>
+      </c>
+      <c r="F30" s="47">
         <f t="shared" ref="F30:F46" si="0">E30/2</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="60">
+        <v>18</v>
+      </c>
+      <c r="G30" s="48">
         <f>F30/2</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="61">
+        <v>9</v>
+      </c>
+      <c r="H30" s="49">
         <f t="shared" ref="H30:H46" si="1">F30/3</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="60">
+        <v>6</v>
+      </c>
+      <c r="I30" s="48">
         <f t="shared" ref="I30:I46" si="2">F30/4</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="61">
+        <v>4.5</v>
+      </c>
+      <c r="J30" s="49">
         <f t="shared" ref="J30:J31" si="3">F30/5</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="61">
+        <v>3.6</v>
+      </c>
+      <c r="K30" s="49">
         <f t="shared" ref="K30:K31" si="4">F30/6</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="61">
+        <v>3</v>
+      </c>
+      <c r="L30" s="49">
         <f t="shared" ref="L30:L31" si="5">F30/7</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="60">
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="M30" s="48">
         <f t="shared" ref="M30:M31" si="6">F30/8</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="61">
+        <v>2.25</v>
+      </c>
+      <c r="N30" s="49">
         <f t="shared" ref="N30:N31" si="7">F30/9</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="61">
+        <v>2</v>
+      </c>
+      <c r="O30" s="49">
         <f t="shared" ref="O30:O31" si="8">F30/10</f>
-        <v>0</v>
-      </c>
-      <c r="P30" s="61">
+        <v>1.8</v>
+      </c>
+      <c r="P30" s="49">
         <f t="shared" ref="P30:P31" si="9">F30/11</f>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="67">
+        <v>1.6363636363636365</v>
+      </c>
+      <c r="Q30" s="55">
         <f t="shared" ref="Q30:Q31" si="10">F30/12</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" s="11"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="58">
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="46">
         <f>C31+D31</f>
         <v>0</v>
       </c>
-      <c r="F31" s="59">
+      <c r="F31" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="60">
+      <c r="G31" s="48">
         <f>F31/2</f>
         <v>0</v>
       </c>
-      <c r="H31" s="61">
+      <c r="H31" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I31" s="60">
+      <c r="I31" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J31" s="61">
+      <c r="J31" s="49">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K31" s="61">
+      <c r="K31" s="49">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L31" s="61">
+      <c r="L31" s="49">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M31" s="60">
+      <c r="M31" s="48">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N31" s="61">
+      <c r="N31" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O31" s="61">
+      <c r="O31" s="49">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P31" s="61">
+      <c r="P31" s="49">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="67">
+      <c r="Q31" s="55">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="11"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="58">
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="46">
         <f t="shared" ref="E32:E46" si="11">C32+D32</f>
         <v>0</v>
       </c>
-      <c r="F32" s="59">
+      <c r="F32" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" s="70">
+      <c r="G32" s="58">
         <f>F32/2</f>
         <v>0</v>
       </c>
-      <c r="H32" s="71">
+      <c r="H32" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32" s="70">
+      <c r="I32" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J32" s="71">
+      <c r="J32" s="59">
         <f t="shared" ref="J32" si="12">F32/5</f>
         <v>0</v>
       </c>
-      <c r="K32" s="71">
+      <c r="K32" s="59">
         <f t="shared" ref="K32" si="13">F32/6</f>
         <v>0</v>
       </c>
-      <c r="L32" s="71">
+      <c r="L32" s="59">
         <f t="shared" ref="L32" si="14">F32/7</f>
         <v>0</v>
       </c>
-      <c r="M32" s="70">
+      <c r="M32" s="58">
         <f t="shared" ref="M32" si="15">F32/8</f>
         <v>0</v>
       </c>
-      <c r="N32" s="71">
+      <c r="N32" s="59">
         <f t="shared" ref="N32" si="16">F32/9</f>
         <v>0</v>
       </c>
-      <c r="O32" s="71">
+      <c r="O32" s="59">
         <f t="shared" ref="O32" si="17">F32/10</f>
         <v>0</v>
       </c>
-      <c r="P32" s="71">
+      <c r="P32" s="59">
         <f t="shared" ref="P32" si="18">F32/11</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="72">
+      <c r="Q32" s="60">
         <f t="shared" ref="Q32" si="19">F32/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="11"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="58">
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F33" s="59">
+      <c r="F33" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G33" s="70">
+      <c r="G33" s="58">
         <f t="shared" ref="G33:G34" si="20">F33/2</f>
         <v>0</v>
       </c>
-      <c r="H33" s="71">
+      <c r="H33" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I33" s="70">
+      <c r="I33" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J33" s="71">
+      <c r="J33" s="59">
         <f t="shared" ref="J33:J38" si="21">F33/5</f>
         <v>0</v>
       </c>
-      <c r="K33" s="71">
+      <c r="K33" s="59">
         <f t="shared" ref="K33:K38" si="22">F33/6</f>
         <v>0</v>
       </c>
-      <c r="L33" s="71">
+      <c r="L33" s="59">
         <f t="shared" ref="L33:L38" si="23">F33/7</f>
         <v>0</v>
       </c>
-      <c r="M33" s="70">
+      <c r="M33" s="58">
         <f t="shared" ref="M33:M38" si="24">F33/8</f>
         <v>0</v>
       </c>
-      <c r="N33" s="71">
+      <c r="N33" s="59">
         <f t="shared" ref="N33:N38" si="25">F33/9</f>
         <v>0</v>
       </c>
-      <c r="O33" s="71">
+      <c r="O33" s="59">
         <f t="shared" ref="O33:O38" si="26">F33/10</f>
         <v>0</v>
       </c>
-      <c r="P33" s="71">
+      <c r="P33" s="59">
         <f t="shared" ref="P33:P38" si="27">F33/11</f>
         <v>0</v>
       </c>
-      <c r="Q33" s="72">
+      <c r="Q33" s="60">
         <f t="shared" ref="Q33:Q38" si="28">F33/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="11"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="58">
+      <c r="C34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F34" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G34" s="70">
+      <c r="G34" s="58">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="H34" s="71">
+      <c r="H34" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I34" s="70">
+      <c r="I34" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J34" s="71">
+      <c r="J34" s="59">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="K34" s="71">
+      <c r="K34" s="59">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="L34" s="71">
+      <c r="L34" s="59">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="M34" s="70">
+      <c r="M34" s="58">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="N34" s="71">
+      <c r="N34" s="59">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="O34" s="71">
+      <c r="O34" s="59">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P34" s="71">
+      <c r="P34" s="59">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="72">
+      <c r="Q34" s="60">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="11"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="58">
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="60">
+      <c r="G35" s="48">
         <f>F35/2</f>
         <v>0</v>
       </c>
-      <c r="H35" s="61">
+      <c r="H35" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I35" s="60">
+      <c r="I35" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J35" s="61">
+      <c r="J35" s="49">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="K35" s="61">
+      <c r="K35" s="49">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="L35" s="61">
+      <c r="L35" s="49">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="M35" s="60">
+      <c r="M35" s="48">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="N35" s="61">
+      <c r="N35" s="49">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="O35" s="61">
+      <c r="O35" s="49">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P35" s="61">
+      <c r="P35" s="49">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="Q35" s="67">
+      <c r="Q35" s="55">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="11"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="58">
+      <c r="C36" s="56"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F36" s="59">
+      <c r="F36" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="60">
+      <c r="G36" s="48">
         <f>F36/2</f>
         <v>0</v>
       </c>
-      <c r="H36" s="61">
+      <c r="H36" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I36" s="60">
+      <c r="I36" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J36" s="61">
+      <c r="J36" s="49">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="K36" s="61">
+      <c r="K36" s="49">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="L36" s="61">
+      <c r="L36" s="49">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="M36" s="60">
+      <c r="M36" s="48">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="N36" s="61">
+      <c r="N36" s="49">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="O36" s="61">
+      <c r="O36" s="49">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P36" s="61">
+      <c r="P36" s="49">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="Q36" s="67">
+      <c r="Q36" s="55">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="58">
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F37" s="59">
+      <c r="F37" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G37" s="60">
+      <c r="G37" s="48">
         <f>F37/2</f>
         <v>0</v>
       </c>
-      <c r="H37" s="61">
+      <c r="H37" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I37" s="60">
+      <c r="I37" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J37" s="61">
+      <c r="J37" s="49">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="K37" s="61">
+      <c r="K37" s="49">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="L37" s="61">
+      <c r="L37" s="49">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="M37" s="60">
+      <c r="M37" s="48">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="N37" s="61">
+      <c r="N37" s="49">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="O37" s="61">
+      <c r="O37" s="49">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P37" s="61">
+      <c r="P37" s="49">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="Q37" s="67">
+      <c r="Q37" s="55">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="11"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="58">
+      <c r="C38" s="56"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F38" s="59">
+      <c r="F38" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G38" s="70">
+      <c r="G38" s="58">
         <f>F38/2</f>
         <v>0</v>
       </c>
-      <c r="H38" s="71">
+      <c r="H38" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I38" s="70">
+      <c r="I38" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J38" s="71">
+      <c r="J38" s="59">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="K38" s="71">
+      <c r="K38" s="59">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="L38" s="71">
+      <c r="L38" s="59">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="M38" s="70">
+      <c r="M38" s="58">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="N38" s="71">
+      <c r="N38" s="59">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="O38" s="71">
+      <c r="O38" s="59">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P38" s="71">
+      <c r="P38" s="59">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="Q38" s="72">
+      <c r="Q38" s="60">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="11"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="58">
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F39" s="59">
+      <c r="F39" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G39" s="70">
+      <c r="G39" s="58">
         <f t="shared" ref="G39:G40" si="29">F39/2</f>
         <v>0</v>
       </c>
-      <c r="H39" s="71">
+      <c r="H39" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I39" s="70">
+      <c r="I39" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J39" s="71">
+      <c r="J39" s="59">
         <f t="shared" ref="J39:J46" si="30">F39/5</f>
         <v>0</v>
       </c>
-      <c r="K39" s="71">
+      <c r="K39" s="59">
         <f t="shared" ref="K39:K46" si="31">F39/6</f>
         <v>0</v>
       </c>
-      <c r="L39" s="71">
+      <c r="L39" s="59">
         <f t="shared" ref="L39:L46" si="32">F39/7</f>
         <v>0</v>
       </c>
-      <c r="M39" s="70">
+      <c r="M39" s="58">
         <f t="shared" ref="M39:M46" si="33">F39/8</f>
         <v>0</v>
       </c>
-      <c r="N39" s="71">
+      <c r="N39" s="59">
         <f t="shared" ref="N39:N46" si="34">F39/9</f>
         <v>0</v>
       </c>
-      <c r="O39" s="71">
+      <c r="O39" s="59">
         <f t="shared" ref="O39:O46" si="35">F39/10</f>
         <v>0</v>
       </c>
-      <c r="P39" s="71">
+      <c r="P39" s="59">
         <f t="shared" ref="P39:P46" si="36">F39/11</f>
         <v>0</v>
       </c>
-      <c r="Q39" s="72">
+      <c r="Q39" s="60">
         <f t="shared" ref="Q39:Q46" si="37">F39/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="11"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="58">
+      <c r="C40" s="56"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G40" s="70">
+      <c r="G40" s="58">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="H40" s="71">
+      <c r="H40" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I40" s="70">
+      <c r="I40" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J40" s="71">
+      <c r="J40" s="59">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K40" s="71">
+      <c r="K40" s="59">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L40" s="71">
+      <c r="L40" s="59">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M40" s="70">
+      <c r="M40" s="58">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N40" s="71">
+      <c r="N40" s="59">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O40" s="71">
+      <c r="O40" s="59">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P40" s="71">
+      <c r="P40" s="59">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q40" s="72">
+      <c r="Q40" s="60">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B41" s="11"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="58">
+      <c r="C41" s="56"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F41" s="59">
+      <c r="F41" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G41" s="60">
+      <c r="G41" s="48">
         <f>F41/2</f>
         <v>0</v>
       </c>
-      <c r="H41" s="61">
+      <c r="H41" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I41" s="60">
+      <c r="I41" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J41" s="61">
+      <c r="J41" s="49">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K41" s="61">
+      <c r="K41" s="49">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L41" s="61">
+      <c r="L41" s="49">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M41" s="60">
+      <c r="M41" s="48">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N41" s="61">
+      <c r="N41" s="49">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O41" s="61">
+      <c r="O41" s="49">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P41" s="61">
+      <c r="P41" s="49">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="67">
+      <c r="Q41" s="55">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="11"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="58">
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F42" s="59">
+      <c r="F42" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G42" s="60">
+      <c r="G42" s="48">
         <f>F42/2</f>
         <v>0</v>
       </c>
-      <c r="H42" s="61">
+      <c r="H42" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I42" s="60">
+      <c r="I42" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J42" s="61">
+      <c r="J42" s="49">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K42" s="61">
+      <c r="K42" s="49">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L42" s="61">
+      <c r="L42" s="49">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M42" s="60">
+      <c r="M42" s="48">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N42" s="61">
+      <c r="N42" s="49">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O42" s="61">
+      <c r="O42" s="49">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P42" s="61">
+      <c r="P42" s="49">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="67">
+      <c r="Q42" s="55">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B43" s="11"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="58">
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F43" s="59">
+      <c r="F43" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G43" s="60">
+      <c r="G43" s="48">
         <f>F43/2</f>
         <v>0</v>
       </c>
-      <c r="H43" s="61">
+      <c r="H43" s="49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I43" s="60">
+      <c r="I43" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J43" s="61">
+      <c r="J43" s="49">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K43" s="61">
+      <c r="K43" s="49">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L43" s="61">
+      <c r="L43" s="49">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M43" s="60">
+      <c r="M43" s="48">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N43" s="61">
+      <c r="N43" s="49">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O43" s="61">
+      <c r="O43" s="49">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P43" s="61">
+      <c r="P43" s="49">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="67">
+      <c r="Q43" s="55">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="11"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="58">
+      <c r="C44" s="56"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F44" s="59">
+      <c r="F44" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G44" s="70">
+      <c r="G44" s="58">
         <f>F44/2</f>
         <v>0</v>
       </c>
-      <c r="H44" s="71">
+      <c r="H44" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I44" s="70">
+      <c r="I44" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J44" s="71">
+      <c r="J44" s="59">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K44" s="71">
+      <c r="K44" s="59">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L44" s="71">
+      <c r="L44" s="59">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M44" s="70">
+      <c r="M44" s="58">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N44" s="71">
+      <c r="N44" s="59">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O44" s="71">
+      <c r="O44" s="59">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P44" s="71">
+      <c r="P44" s="59">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="72">
+      <c r="Q44" s="60">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B45" s="11"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="58">
+      <c r="C45" s="56"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F45" s="59">
+      <c r="F45" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G45" s="70">
+      <c r="G45" s="58">
         <f t="shared" ref="G45:G46" si="38">F45/2</f>
         <v>0</v>
       </c>
-      <c r="H45" s="71">
+      <c r="H45" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I45" s="70">
+      <c r="I45" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J45" s="71">
+      <c r="J45" s="59">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K45" s="71">
+      <c r="K45" s="59">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L45" s="71">
+      <c r="L45" s="59">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M45" s="70">
+      <c r="M45" s="58">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N45" s="71">
+      <c r="N45" s="59">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O45" s="71">
+      <c r="O45" s="59">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P45" s="71">
+      <c r="P45" s="59">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q45" s="72">
+      <c r="Q45" s="60">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B46" s="12"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="73">
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="61">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F46" s="74">
+      <c r="F46" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G46" s="75">
+      <c r="G46" s="63">
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="H46" s="76">
+      <c r="H46" s="64">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I46" s="75">
+      <c r="I46" s="63">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J46" s="76">
+      <c r="J46" s="64">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K46" s="76">
+      <c r="K46" s="64">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L46" s="76">
+      <c r="L46" s="64">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M46" s="75">
+      <c r="M46" s="63">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N46" s="76">
+      <c r="N46" s="64">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O46" s="76">
+      <c r="O46" s="64">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="P46" s="76">
+      <c r="P46" s="64">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="Q46" s="77">
+      <c r="Q46" s="65">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
@@ -2534,1030 +2652,1032 @@
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
-      <c r="C53" s="56">
+      <c r="C53" s="44">
         <v>26</v>
       </c>
-      <c r="D53" s="57">
+      <c r="D53" s="45">
         <v>0.25</v>
       </c>
-      <c r="E53" s="79">
+      <c r="E53" s="67">
         <f>C53+D53</f>
         <v>26.25</v>
       </c>
-      <c r="F53" s="80">
+      <c r="F53" s="68">
         <f>E53</f>
         <v>26.25</v>
       </c>
-      <c r="G53" s="60">
+      <c r="G53" s="48">
         <f>F53/2</f>
         <v>13.125</v>
       </c>
-      <c r="H53" s="61">
+      <c r="H53" s="49">
         <f>F53/3</f>
         <v>8.75</v>
       </c>
-      <c r="I53" s="60">
+      <c r="I53" s="48">
         <f>F53/4</f>
         <v>6.5625</v>
       </c>
-      <c r="J53" s="61">
+      <c r="J53" s="49">
         <f>F53/5</f>
         <v>5.25</v>
       </c>
-      <c r="K53" s="61">
+      <c r="K53" s="49">
         <f>F53/6</f>
         <v>4.375</v>
       </c>
-      <c r="L53" s="61">
+      <c r="L53" s="49">
         <f>F53/7</f>
         <v>3.75</v>
       </c>
-      <c r="M53" s="60">
+      <c r="M53" s="48">
         <f>F53/8</f>
         <v>3.28125</v>
       </c>
-      <c r="N53" s="61">
+      <c r="N53" s="49">
         <f>F53/9</f>
         <v>2.9166666666666665</v>
       </c>
-      <c r="O53" s="61">
+      <c r="O53" s="49">
         <f>F53/10</f>
         <v>2.625</v>
       </c>
-      <c r="P53" s="61">
+      <c r="P53" s="49">
         <f>F53/11</f>
         <v>2.3863636363636362</v>
       </c>
-      <c r="Q53" s="67">
+      <c r="Q53" s="55">
         <f>F53/12</f>
         <v>2.1875</v>
       </c>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B54" s="11"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="69"/>
-      <c r="E54" s="79">
+      <c r="C54" s="56">
+        <v>36</v>
+      </c>
+      <c r="D54" s="57"/>
+      <c r="E54" s="67">
         <f>C54+D54</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="80">
+        <v>36</v>
+      </c>
+      <c r="F54" s="68">
         <f>E54</f>
-        <v>0</v>
-      </c>
-      <c r="G54" s="60">
+        <v>36</v>
+      </c>
+      <c r="G54" s="48">
         <f>F54/2</f>
-        <v>0</v>
-      </c>
-      <c r="H54" s="61">
+        <v>18</v>
+      </c>
+      <c r="H54" s="49">
         <f>F54/3</f>
-        <v>0</v>
-      </c>
-      <c r="I54" s="60">
+        <v>12</v>
+      </c>
+      <c r="I54" s="48">
         <f>F54/4</f>
-        <v>0</v>
-      </c>
-      <c r="J54" s="61">
+        <v>9</v>
+      </c>
+      <c r="J54" s="49">
         <f>F54/5</f>
-        <v>0</v>
-      </c>
-      <c r="K54" s="61">
+        <v>7.2</v>
+      </c>
+      <c r="K54" s="49">
         <f>F54/6</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="61">
+        <v>6</v>
+      </c>
+      <c r="L54" s="49">
         <f>F54/7</f>
-        <v>0</v>
-      </c>
-      <c r="M54" s="60">
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="M54" s="48">
         <f>F54/8</f>
-        <v>0</v>
-      </c>
-      <c r="N54" s="61">
+        <v>4.5</v>
+      </c>
+      <c r="N54" s="49">
         <f>F54/9</f>
-        <v>0</v>
-      </c>
-      <c r="O54" s="61">
+        <v>4</v>
+      </c>
+      <c r="O54" s="49">
         <f>F54/10</f>
-        <v>0</v>
-      </c>
-      <c r="P54" s="61">
+        <v>3.6</v>
+      </c>
+      <c r="P54" s="49">
         <f>F54/11</f>
-        <v>0</v>
-      </c>
-      <c r="Q54" s="67">
+        <v>3.2727272727272729</v>
+      </c>
+      <c r="Q54" s="55">
         <f>F54/12</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B55" s="11"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="79">
+      <c r="C55" s="56"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="67">
         <f>C55+D55</f>
         <v>0</v>
       </c>
-      <c r="F55" s="80">
+      <c r="F55" s="68">
         <f>E55</f>
         <v>0</v>
       </c>
-      <c r="G55" s="60">
+      <c r="G55" s="48">
         <f>F55/2</f>
         <v>0</v>
       </c>
-      <c r="H55" s="61">
+      <c r="H55" s="49">
         <f>F55/3</f>
         <v>0</v>
       </c>
-      <c r="I55" s="60">
+      <c r="I55" s="48">
         <f>F55/4</f>
         <v>0</v>
       </c>
-      <c r="J55" s="61">
+      <c r="J55" s="49">
         <f>F55/5</f>
         <v>0</v>
       </c>
-      <c r="K55" s="61">
+      <c r="K55" s="49">
         <f>F55/6</f>
         <v>0</v>
       </c>
-      <c r="L55" s="61">
+      <c r="L55" s="49">
         <f>F55/7</f>
         <v>0</v>
       </c>
-      <c r="M55" s="60">
+      <c r="M55" s="48">
         <f>F55/8</f>
         <v>0</v>
       </c>
-      <c r="N55" s="61">
+      <c r="N55" s="49">
         <f>F55/9</f>
         <v>0</v>
       </c>
-      <c r="O55" s="61">
+      <c r="O55" s="49">
         <f>F55/10</f>
         <v>0</v>
       </c>
-      <c r="P55" s="61">
+      <c r="P55" s="49">
         <f>F55/11</f>
         <v>0</v>
       </c>
-      <c r="Q55" s="67">
+      <c r="Q55" s="55">
         <f>F55/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B56" s="11"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="79">
+      <c r="C56" s="56"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="67">
         <f>C56+D56</f>
         <v>0</v>
       </c>
-      <c r="F56" s="80">
+      <c r="F56" s="68">
         <f>E56</f>
         <v>0</v>
       </c>
-      <c r="G56" s="70">
+      <c r="G56" s="58">
         <f>F56/2</f>
         <v>0</v>
       </c>
-      <c r="H56" s="71">
+      <c r="H56" s="59">
         <f>F56/3</f>
         <v>0</v>
       </c>
-      <c r="I56" s="70">
+      <c r="I56" s="58">
         <f>F56/4</f>
         <v>0</v>
       </c>
-      <c r="J56" s="71">
+      <c r="J56" s="59">
         <f>F56/5</f>
         <v>0</v>
       </c>
-      <c r="K56" s="71">
+      <c r="K56" s="59">
         <f>F56/6</f>
         <v>0</v>
       </c>
-      <c r="L56" s="71">
+      <c r="L56" s="59">
         <f>F56/7</f>
         <v>0</v>
       </c>
-      <c r="M56" s="70">
+      <c r="M56" s="58">
         <f>F56/8</f>
         <v>0</v>
       </c>
-      <c r="N56" s="71">
+      <c r="N56" s="59">
         <f>F56/9</f>
         <v>0</v>
       </c>
-      <c r="O56" s="71">
+      <c r="O56" s="59">
         <f>F56/10</f>
         <v>0</v>
       </c>
-      <c r="P56" s="71">
+      <c r="P56" s="59">
         <f>F56/11</f>
         <v>0</v>
       </c>
-      <c r="Q56" s="72">
+      <c r="Q56" s="60">
         <f>F56/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B57" s="11"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="79">
+      <c r="C57" s="56"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="67">
         <f t="shared" ref="E57:E62" si="39">C57+D57</f>
         <v>0</v>
       </c>
-      <c r="F57" s="80">
+      <c r="F57" s="68">
         <f t="shared" ref="F57:F70" si="40">E57</f>
         <v>0</v>
       </c>
-      <c r="G57" s="70">
+      <c r="G57" s="58">
         <f t="shared" ref="G57:G70" si="41">F57/2</f>
         <v>0</v>
       </c>
-      <c r="H57" s="71">
+      <c r="H57" s="59">
         <f t="shared" ref="H57:H62" si="42">F57/3</f>
         <v>0</v>
       </c>
-      <c r="I57" s="70">
+      <c r="I57" s="58">
         <f t="shared" ref="I57:I62" si="43">F57/4</f>
         <v>0</v>
       </c>
-      <c r="J57" s="71">
+      <c r="J57" s="59">
         <f t="shared" ref="J57:J62" si="44">F57/5</f>
         <v>0</v>
       </c>
-      <c r="K57" s="71">
+      <c r="K57" s="59">
         <f t="shared" ref="K57:K62" si="45">F57/6</f>
         <v>0</v>
       </c>
-      <c r="L57" s="71">
+      <c r="L57" s="59">
         <f t="shared" ref="L57:L62" si="46">F57/7</f>
         <v>0</v>
       </c>
-      <c r="M57" s="70">
+      <c r="M57" s="58">
         <f t="shared" ref="M57:M62" si="47">F57/8</f>
         <v>0</v>
       </c>
-      <c r="N57" s="71">
+      <c r="N57" s="59">
         <f t="shared" ref="N57:N62" si="48">F57/9</f>
         <v>0</v>
       </c>
-      <c r="O57" s="71">
+      <c r="O57" s="59">
         <f t="shared" ref="O57:O62" si="49">F57/10</f>
         <v>0</v>
       </c>
-      <c r="P57" s="71">
+      <c r="P57" s="59">
         <f t="shared" ref="P57:P62" si="50">F57/11</f>
         <v>0</v>
       </c>
-      <c r="Q57" s="72">
+      <c r="Q57" s="60">
         <f t="shared" ref="Q57:Q62" si="51">F57/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B58" s="11"/>
-      <c r="C58" s="68"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="79">
+      <c r="C58" s="56"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="67">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="F58" s="80">
+      <c r="F58" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G58" s="70">
+      <c r="G58" s="58">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H58" s="71">
+      <c r="H58" s="59">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="I58" s="70">
+      <c r="I58" s="58">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="J58" s="71">
+      <c r="J58" s="59">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="K58" s="71">
+      <c r="K58" s="59">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="L58" s="71">
+      <c r="L58" s="59">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="M58" s="70">
+      <c r="M58" s="58">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="N58" s="71">
+      <c r="N58" s="59">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="O58" s="71">
+      <c r="O58" s="59">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="P58" s="71">
+      <c r="P58" s="59">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="Q58" s="72">
+      <c r="Q58" s="60">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B59" s="11"/>
-      <c r="C59" s="68"/>
-      <c r="D59" s="69"/>
-      <c r="E59" s="79">
+      <c r="C59" s="56"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="67">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="F59" s="80">
+      <c r="F59" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G59" s="60">
+      <c r="G59" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H59" s="61">
+      <c r="H59" s="49">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="I59" s="60">
+      <c r="I59" s="48">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="J59" s="61">
+      <c r="J59" s="49">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="K59" s="61">
+      <c r="K59" s="49">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="L59" s="61">
+      <c r="L59" s="49">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="M59" s="60">
+      <c r="M59" s="48">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="N59" s="61">
+      <c r="N59" s="49">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="O59" s="61">
+      <c r="O59" s="49">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="P59" s="61">
+      <c r="P59" s="49">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="Q59" s="67">
+      <c r="Q59" s="55">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B60" s="11"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="69"/>
-      <c r="E60" s="79">
+      <c r="C60" s="56"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="67">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="F60" s="80">
+      <c r="F60" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G60" s="60">
+      <c r="G60" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H60" s="61">
+      <c r="H60" s="49">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="I60" s="60">
+      <c r="I60" s="48">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="J60" s="61">
+      <c r="J60" s="49">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="K60" s="61">
+      <c r="K60" s="49">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="L60" s="61">
+      <c r="L60" s="49">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="M60" s="60">
+      <c r="M60" s="48">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="N60" s="61">
+      <c r="N60" s="49">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="O60" s="61">
+      <c r="O60" s="49">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="P60" s="61">
+      <c r="P60" s="49">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="Q60" s="67">
+      <c r="Q60" s="55">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B61" s="11"/>
-      <c r="C61" s="68"/>
-      <c r="D61" s="69"/>
-      <c r="E61" s="79">
+      <c r="C61" s="56"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="67">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="F61" s="80">
+      <c r="F61" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G61" s="60">
+      <c r="G61" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H61" s="61">
+      <c r="H61" s="49">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="I61" s="60">
+      <c r="I61" s="48">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="J61" s="61">
+      <c r="J61" s="49">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="K61" s="61">
+      <c r="K61" s="49">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="L61" s="61">
+      <c r="L61" s="49">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="M61" s="60">
+      <c r="M61" s="48">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="N61" s="61">
+      <c r="N61" s="49">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="O61" s="61">
+      <c r="O61" s="49">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="P61" s="61">
+      <c r="P61" s="49">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="Q61" s="67">
+      <c r="Q61" s="55">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B62" s="11"/>
-      <c r="C62" s="68"/>
-      <c r="D62" s="69"/>
-      <c r="E62" s="79">
+      <c r="C62" s="56"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="67">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="F62" s="80">
+      <c r="F62" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G62" s="70">
+      <c r="G62" s="58">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H62" s="71">
+      <c r="H62" s="59">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="I62" s="70">
+      <c r="I62" s="58">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="J62" s="71">
+      <c r="J62" s="59">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="K62" s="71">
+      <c r="K62" s="59">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="L62" s="71">
+      <c r="L62" s="59">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="M62" s="70">
+      <c r="M62" s="58">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="N62" s="71">
+      <c r="N62" s="59">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="O62" s="71">
+      <c r="O62" s="59">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="P62" s="71">
+      <c r="P62" s="59">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="Q62" s="72">
+      <c r="Q62" s="60">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B63" s="11"/>
-      <c r="C63" s="68"/>
-      <c r="D63" s="69"/>
-      <c r="E63" s="79">
+      <c r="C63" s="56"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="67">
         <f t="shared" ref="E63:E70" si="52">C63+D63</f>
         <v>0</v>
       </c>
-      <c r="F63" s="80">
+      <c r="F63" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G63" s="70">
+      <c r="G63" s="58">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H63" s="71">
+      <c r="H63" s="59">
         <f t="shared" ref="H63:H70" si="53">F63/3</f>
         <v>0</v>
       </c>
-      <c r="I63" s="70">
+      <c r="I63" s="58">
         <f t="shared" ref="I63:I70" si="54">F63/4</f>
         <v>0</v>
       </c>
-      <c r="J63" s="71">
+      <c r="J63" s="59">
         <f t="shared" ref="J63:J70" si="55">F63/5</f>
         <v>0</v>
       </c>
-      <c r="K63" s="71">
+      <c r="K63" s="59">
         <f t="shared" ref="K63:K70" si="56">F63/6</f>
         <v>0</v>
       </c>
-      <c r="L63" s="71">
+      <c r="L63" s="59">
         <f t="shared" ref="L63:L70" si="57">F63/7</f>
         <v>0</v>
       </c>
-      <c r="M63" s="70">
+      <c r="M63" s="58">
         <f t="shared" ref="M63:M70" si="58">F63/8</f>
         <v>0</v>
       </c>
-      <c r="N63" s="71">
+      <c r="N63" s="59">
         <f t="shared" ref="N63:N70" si="59">F63/9</f>
         <v>0</v>
       </c>
-      <c r="O63" s="71">
+      <c r="O63" s="59">
         <f t="shared" ref="O63:O70" si="60">F63/10</f>
         <v>0</v>
       </c>
-      <c r="P63" s="71">
+      <c r="P63" s="59">
         <f t="shared" ref="P63:P70" si="61">F63/11</f>
         <v>0</v>
       </c>
-      <c r="Q63" s="72">
+      <c r="Q63" s="60">
         <f t="shared" ref="Q63:Q70" si="62">F63/12</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B64" s="11"/>
-      <c r="C64" s="68"/>
-      <c r="D64" s="69"/>
-      <c r="E64" s="79">
+      <c r="C64" s="56"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="67">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F64" s="80">
+      <c r="F64" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G64" s="70">
+      <c r="G64" s="58">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H64" s="71">
+      <c r="H64" s="59">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I64" s="70">
+      <c r="I64" s="58">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J64" s="71">
+      <c r="J64" s="59">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K64" s="71">
+      <c r="K64" s="59">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L64" s="71">
+      <c r="L64" s="59">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M64" s="70">
+      <c r="M64" s="58">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N64" s="71">
+      <c r="N64" s="59">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O64" s="71">
+      <c r="O64" s="59">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P64" s="71">
+      <c r="P64" s="59">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q64" s="72">
+      <c r="Q64" s="60">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B65" s="11"/>
-      <c r="C65" s="68"/>
-      <c r="D65" s="69"/>
-      <c r="E65" s="79">
+      <c r="C65" s="56"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="67">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F65" s="80">
+      <c r="F65" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G65" s="60">
+      <c r="G65" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H65" s="61">
+      <c r="H65" s="49">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I65" s="60">
+      <c r="I65" s="48">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J65" s="61">
+      <c r="J65" s="49">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K65" s="61">
+      <c r="K65" s="49">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L65" s="61">
+      <c r="L65" s="49">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M65" s="60">
+      <c r="M65" s="48">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N65" s="61">
+      <c r="N65" s="49">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O65" s="61">
+      <c r="O65" s="49">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P65" s="61">
+      <c r="P65" s="49">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q65" s="67">
+      <c r="Q65" s="55">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B66" s="11"/>
-      <c r="C66" s="68"/>
-      <c r="D66" s="69"/>
-      <c r="E66" s="79">
+      <c r="C66" s="56"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="67">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F66" s="80">
+      <c r="F66" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G66" s="60">
+      <c r="G66" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H66" s="61">
+      <c r="H66" s="49">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I66" s="60">
+      <c r="I66" s="48">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J66" s="61">
+      <c r="J66" s="49">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K66" s="61">
+      <c r="K66" s="49">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L66" s="61">
+      <c r="L66" s="49">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M66" s="60">
+      <c r="M66" s="48">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N66" s="61">
+      <c r="N66" s="49">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O66" s="61">
+      <c r="O66" s="49">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P66" s="61">
+      <c r="P66" s="49">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q66" s="67">
+      <c r="Q66" s="55">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B67" s="11"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="69"/>
-      <c r="E67" s="79">
+      <c r="C67" s="56"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="67">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F67" s="80">
+      <c r="F67" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G67" s="60">
+      <c r="G67" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H67" s="61">
+      <c r="H67" s="49">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I67" s="60">
+      <c r="I67" s="48">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J67" s="61">
+      <c r="J67" s="49">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K67" s="61">
+      <c r="K67" s="49">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L67" s="61">
+      <c r="L67" s="49">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M67" s="60">
+      <c r="M67" s="48">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N67" s="61">
+      <c r="N67" s="49">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O67" s="61">
+      <c r="O67" s="49">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P67" s="61">
+      <c r="P67" s="49">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q67" s="67">
+      <c r="Q67" s="55">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B68" s="11"/>
-      <c r="C68" s="68"/>
-      <c r="D68" s="69"/>
-      <c r="E68" s="79">
+      <c r="C68" s="56"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="67">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F68" s="80">
+      <c r="F68" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G68" s="70">
+      <c r="G68" s="58">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H68" s="71">
+      <c r="H68" s="59">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I68" s="70">
+      <c r="I68" s="58">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J68" s="71">
+      <c r="J68" s="59">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K68" s="71">
+      <c r="K68" s="59">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L68" s="71">
+      <c r="L68" s="59">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M68" s="70">
+      <c r="M68" s="58">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N68" s="71">
+      <c r="N68" s="59">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O68" s="71">
+      <c r="O68" s="59">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P68" s="71">
+      <c r="P68" s="59">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q68" s="72">
+      <c r="Q68" s="60">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B69" s="11"/>
-      <c r="C69" s="68"/>
-      <c r="D69" s="69"/>
-      <c r="E69" s="79">
+      <c r="C69" s="56"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="67">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F69" s="80">
+      <c r="F69" s="68">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G69" s="70">
+      <c r="G69" s="58">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H69" s="71">
+      <c r="H69" s="59">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I69" s="70">
+      <c r="I69" s="58">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J69" s="71">
+      <c r="J69" s="59">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K69" s="71">
+      <c r="K69" s="59">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L69" s="71">
+      <c r="L69" s="59">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M69" s="70">
+      <c r="M69" s="58">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N69" s="71">
+      <c r="N69" s="59">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O69" s="71">
+      <c r="O69" s="59">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P69" s="71">
+      <c r="P69" s="59">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q69" s="72">
+      <c r="Q69" s="60">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B70" s="12"/>
-      <c r="C70" s="62"/>
-      <c r="D70" s="63"/>
-      <c r="E70" s="81">
+      <c r="C70" s="50"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="69">
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="F70" s="82">
+      <c r="F70" s="70">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="G70" s="75">
+      <c r="G70" s="63">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="H70" s="76">
+      <c r="H70" s="64">
         <f t="shared" si="53"/>
         <v>0</v>
       </c>
-      <c r="I70" s="75">
+      <c r="I70" s="63">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="J70" s="76">
+      <c r="J70" s="64">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="K70" s="76">
+      <c r="K70" s="64">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="L70" s="76">
+      <c r="L70" s="64">
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="M70" s="75">
+      <c r="M70" s="63">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="N70" s="76">
+      <c r="N70" s="64">
         <f t="shared" si="59"/>
         <v>0</v>
       </c>
-      <c r="O70" s="76">
+      <c r="O70" s="64">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="P70" s="76">
+      <c r="P70" s="64">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="Q70" s="77">
+      <c r="Q70" s="65">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
@@ -3591,14 +3711,14 @@
       <c r="Z73" s="13"/>
     </row>
     <row r="74" spans="1:26" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B74" s="46" t="s">
+      <c r="B74" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
-      <c r="F74" s="47"/>
-      <c r="G74" s="47"/>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="74"/>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
@@ -3609,10 +3729,10 @@
       <c r="B77" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="53" t="s">
+      <c r="C77" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="53"/>
+      <c r="D77" s="80"/>
       <c r="E77" s="16" t="s">
         <v>13</v>
       </c>
@@ -3633,10 +3753,10 @@
       <c r="B78" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="51">
+      <c r="C78" s="76">
         <v>20.8</v>
       </c>
-      <c r="D78" s="52"/>
+      <c r="D78" s="77"/>
       <c r="E78" s="21">
         <f>C78</f>
         <v>20.8</v>
@@ -3660,8 +3780,8 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B79" s="20"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="55"/>
+      <c r="C79" s="81"/>
+      <c r="D79" s="82"/>
       <c r="E79" s="25"/>
       <c r="F79" s="26"/>
       <c r="G79" s="27"/>
@@ -3692,10 +3812,10 @@
       <c r="B87" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C87" s="50" t="s">
+      <c r="C87" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D87" s="50"/>
+      <c r="D87" s="75"/>
       <c r="E87" s="7" t="s">
         <v>13</v>
       </c>
@@ -3740,10 +3860,10 @@
       <c r="B88" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="51">
+      <c r="C88" s="76">
         <v>106</v>
       </c>
-      <c r="D88" s="52">
+      <c r="D88" s="77">
         <v>0.5</v>
       </c>
       <c r="E88" s="21">
@@ -3801,8 +3921,8 @@
     </row>
     <row r="89" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B89" s="11"/>
-      <c r="C89" s="48"/>
-      <c r="D89" s="49">
+      <c r="C89" s="71"/>
+      <c r="D89" s="72">
         <v>0.5</v>
       </c>
       <c r="E89" s="21">
@@ -3860,8 +3980,8 @@
     </row>
     <row r="90" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B90" s="11"/>
-      <c r="C90" s="48"/>
-      <c r="D90" s="49"/>
+      <c r="C90" s="71"/>
+      <c r="D90" s="72"/>
       <c r="E90" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -3917,8 +4037,8 @@
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B91" s="11"/>
-      <c r="C91" s="48"/>
-      <c r="D91" s="49"/>
+      <c r="C91" s="71"/>
+      <c r="D91" s="72"/>
       <c r="E91" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -3974,8 +4094,8 @@
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B92" s="11"/>
-      <c r="C92" s="48"/>
-      <c r="D92" s="49"/>
+      <c r="C92" s="71"/>
+      <c r="D92" s="72"/>
       <c r="E92" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4031,8 +4151,8 @@
     </row>
     <row r="93" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B93" s="11"/>
-      <c r="C93" s="48"/>
-      <c r="D93" s="49"/>
+      <c r="C93" s="71"/>
+      <c r="D93" s="72"/>
       <c r="E93" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4088,8 +4208,8 @@
     </row>
     <row r="94" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B94" s="11"/>
-      <c r="C94" s="48"/>
-      <c r="D94" s="49"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="72"/>
       <c r="E94" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4145,8 +4265,8 @@
     </row>
     <row r="95" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B95" s="11"/>
-      <c r="C95" s="48"/>
-      <c r="D95" s="49"/>
+      <c r="C95" s="71"/>
+      <c r="D95" s="72"/>
       <c r="E95" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4202,8 +4322,8 @@
     </row>
     <row r="96" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B96" s="11"/>
-      <c r="C96" s="48"/>
-      <c r="D96" s="49"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="72"/>
       <c r="E96" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4259,8 +4379,8 @@
     </row>
     <row r="97" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B97" s="11"/>
-      <c r="C97" s="48"/>
-      <c r="D97" s="49"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="72"/>
       <c r="E97" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4316,8 +4436,8 @@
     </row>
     <row r="98" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B98" s="11"/>
-      <c r="C98" s="48"/>
-      <c r="D98" s="49"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="72"/>
       <c r="E98" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4373,8 +4493,8 @@
     </row>
     <row r="99" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B99" s="11"/>
-      <c r="C99" s="48"/>
-      <c r="D99" s="49"/>
+      <c r="C99" s="71"/>
+      <c r="D99" s="72"/>
       <c r="E99" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4430,8 +4550,8 @@
     </row>
     <row r="100" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B100" s="11"/>
-      <c r="C100" s="48"/>
-      <c r="D100" s="49"/>
+      <c r="C100" s="71"/>
+      <c r="D100" s="72"/>
       <c r="E100" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4487,8 +4607,8 @@
     </row>
     <row r="101" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B101" s="11"/>
-      <c r="C101" s="48"/>
-      <c r="D101" s="49"/>
+      <c r="C101" s="71"/>
+      <c r="D101" s="72"/>
       <c r="E101" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4544,8 +4664,8 @@
     </row>
     <row r="102" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B102" s="11"/>
-      <c r="C102" s="48"/>
-      <c r="D102" s="49"/>
+      <c r="C102" s="71"/>
+      <c r="D102" s="72"/>
       <c r="E102" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4601,8 +4721,8 @@
     </row>
     <row r="103" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B103" s="11"/>
-      <c r="C103" s="48"/>
-      <c r="D103" s="49"/>
+      <c r="C103" s="71"/>
+      <c r="D103" s="72"/>
       <c r="E103" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4658,8 +4778,8 @@
     </row>
     <row r="104" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B104" s="11"/>
-      <c r="C104" s="48"/>
-      <c r="D104" s="49"/>
+      <c r="C104" s="71"/>
+      <c r="D104" s="72"/>
       <c r="E104" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4715,8 +4835,8 @@
     </row>
     <row r="105" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B105" s="12"/>
-      <c r="C105" s="44"/>
-      <c r="D105" s="45"/>
+      <c r="C105" s="78"/>
+      <c r="D105" s="79"/>
       <c r="E105" s="21">
         <f t="shared" si="74"/>
         <v>0</v>
@@ -4779,10 +4899,10 @@
       <c r="B110" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="50" t="s">
+      <c r="C110" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D110" s="50"/>
+      <c r="D110" s="75"/>
       <c r="E110" s="7" t="s">
         <v>13</v>
       </c>
@@ -4825,10 +4945,10 @@
     </row>
     <row r="111" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B111" s="10"/>
-      <c r="C111" s="51">
+      <c r="C111" s="76">
         <v>38.700000000000003</v>
       </c>
-      <c r="D111" s="52">
+      <c r="D111" s="77">
         <v>0.5</v>
       </c>
       <c r="E111" s="21">
@@ -4886,8 +5006,8 @@
     </row>
     <row r="112" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B112" s="11"/>
-      <c r="C112" s="48"/>
-      <c r="D112" s="49"/>
+      <c r="C112" s="71"/>
+      <c r="D112" s="72"/>
       <c r="E112" s="21">
         <f t="shared" ref="E112:E128" si="103">C112</f>
         <v>0</v>
@@ -4943,8 +5063,8 @@
     </row>
     <row r="113" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B113" s="11"/>
-      <c r="C113" s="48"/>
-      <c r="D113" s="49"/>
+      <c r="C113" s="71"/>
+      <c r="D113" s="72"/>
       <c r="E113" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5000,8 +5120,8 @@
     </row>
     <row r="114" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B114" s="11"/>
-      <c r="C114" s="48"/>
-      <c r="D114" s="49"/>
+      <c r="C114" s="71"/>
+      <c r="D114" s="72"/>
       <c r="E114" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5057,8 +5177,8 @@
     </row>
     <row r="115" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B115" s="11"/>
-      <c r="C115" s="48"/>
-      <c r="D115" s="49"/>
+      <c r="C115" s="71"/>
+      <c r="D115" s="72"/>
       <c r="E115" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5114,8 +5234,8 @@
     </row>
     <row r="116" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B116" s="11"/>
-      <c r="C116" s="48"/>
-      <c r="D116" s="49"/>
+      <c r="C116" s="71"/>
+      <c r="D116" s="72"/>
       <c r="E116" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5171,8 +5291,8 @@
     </row>
     <row r="117" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B117" s="11"/>
-      <c r="C117" s="48"/>
-      <c r="D117" s="49"/>
+      <c r="C117" s="71"/>
+      <c r="D117" s="72"/>
       <c r="E117" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5228,8 +5348,8 @@
     </row>
     <row r="118" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B118" s="11"/>
-      <c r="C118" s="48"/>
-      <c r="D118" s="49"/>
+      <c r="C118" s="71"/>
+      <c r="D118" s="72"/>
       <c r="E118" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5285,8 +5405,8 @@
     </row>
     <row r="119" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B119" s="11"/>
-      <c r="C119" s="48"/>
-      <c r="D119" s="49"/>
+      <c r="C119" s="71"/>
+      <c r="D119" s="72"/>
       <c r="E119" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5342,8 +5462,8 @@
     </row>
     <row r="120" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B120" s="11"/>
-      <c r="C120" s="48"/>
-      <c r="D120" s="49"/>
+      <c r="C120" s="71"/>
+      <c r="D120" s="72"/>
       <c r="E120" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5399,8 +5519,8 @@
     </row>
     <row r="121" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B121" s="11"/>
-      <c r="C121" s="48"/>
-      <c r="D121" s="49"/>
+      <c r="C121" s="71"/>
+      <c r="D121" s="72"/>
       <c r="E121" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5456,8 +5576,8 @@
     </row>
     <row r="122" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B122" s="11"/>
-      <c r="C122" s="48"/>
-      <c r="D122" s="49"/>
+      <c r="C122" s="71"/>
+      <c r="D122" s="72"/>
       <c r="E122" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5513,8 +5633,8 @@
     </row>
     <row r="123" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B123" s="11"/>
-      <c r="C123" s="48"/>
-      <c r="D123" s="49"/>
+      <c r="C123" s="71"/>
+      <c r="D123" s="72"/>
       <c r="E123" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5570,8 +5690,8 @@
     </row>
     <row r="124" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B124" s="11"/>
-      <c r="C124" s="48"/>
-      <c r="D124" s="49"/>
+      <c r="C124" s="71"/>
+      <c r="D124" s="72"/>
       <c r="E124" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5627,8 +5747,8 @@
     </row>
     <row r="125" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B125" s="11"/>
-      <c r="C125" s="48"/>
-      <c r="D125" s="49"/>
+      <c r="C125" s="71"/>
+      <c r="D125" s="72"/>
       <c r="E125" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5684,8 +5804,8 @@
     </row>
     <row r="126" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B126" s="11"/>
-      <c r="C126" s="48"/>
-      <c r="D126" s="49"/>
+      <c r="C126" s="71"/>
+      <c r="D126" s="72"/>
       <c r="E126" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5741,8 +5861,8 @@
     </row>
     <row r="127" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B127" s="11"/>
-      <c r="C127" s="48"/>
-      <c r="D127" s="49"/>
+      <c r="C127" s="71"/>
+      <c r="D127" s="72"/>
       <c r="E127" s="21">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5798,8 +5918,8 @@
     </row>
     <row r="128" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B128" s="12"/>
-      <c r="C128" s="44"/>
-      <c r="D128" s="45"/>
+      <c r="C128" s="78"/>
+      <c r="D128" s="79"/>
       <c r="E128" s="33">
         <f t="shared" si="103"/>
         <v>0</v>
@@ -5855,17 +5975,22 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
     <mergeCell ref="C117:D117"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="B74:G74"/>
@@ -5882,22 +6007,17 @@
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>